<commit_message>
update PS2 to make nice for Latex
</commit_message>
<xml_diff>
--- a/Education Economics/data/PS2_tables.xlsx
+++ b/Education Economics/data/PS2_tables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericenglin/Desktop/HKS Classes/EDU A206/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric.englin\Desktop\Github\Data-Science-Assignments\Education Economics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC30D84-549A-B841-8948-A25F43F5A4AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="1300" windowWidth="18820" windowHeight="17440" activeTab="1" xr2:uid="{18A1C4C8-69E0-6844-934B-DC7326961E8F}"/>
+    <workbookView xWindow="-144" yWindow="1296" windowWidth="18816" windowHeight="17436" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>Self-Revelation</t>
   </si>
@@ -193,7 +192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -267,12 +266,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -289,12 +287,12 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -611,36 +609,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F178010F-9F46-7D46-8067-AFDB6C7A0737}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -661,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -684,7 +682,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -707,7 +705,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
@@ -736,7 +734,7 @@
         <v>0.121</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -765,7 +763,7 @@
         <v>-2.2999999999999993E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -786,7 +784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -809,7 +807,7 @@
         <v>0.14299999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -832,7 +830,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -861,7 +859,7 @@
         <v>0.249</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -902,22 +900,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53F89DA-6178-854C-A014-D9328C2C3AF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -934,7 +932,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -953,7 +951,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -972,7 +970,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -991,7 +989,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1010,7 +1008,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1027,7 +1025,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1044,7 +1042,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
     </row>
   </sheetData>
@@ -1053,16 +1051,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26DE520-413E-4F4F-85F0-4C8CB1DDCA26}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>36</v>
@@ -1083,7 +1081,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -1106,7 +1104,7 @@
         <v>0.14299999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1129,7 +1127,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1138,7 +1136,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1153,29 +1151,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7560E4F-B669-604F-8BC6-B94BCA5274C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:O24"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.69921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.69921875" customWidth="1"/>
     <col min="10" max="11" width="11.5" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.296875" customWidth="1"/>
+    <col min="15" max="15" width="18.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -1201,10 +1199,10 @@
       <c r="I4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -1214,47 +1212,47 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>0.77</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>26350</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>26350</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <f>C5*(1+(B5)/100)</f>
         <v>26552.895</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <f>E5</f>
         <v>26552.895</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <f>E5-D5</f>
         <v>202.89500000000044</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <f>G5</f>
         <v>202.89500000000044</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>0</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <f>G5/((1.03)^2)</f>
         <v>191.2479969836935</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <f>H5/((1.03)^3)</f>
         <v>185.6776669744597</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="8">
         <f>K5+J5</f>
         <v>376.92566395815322</v>
       </c>
@@ -1270,47 +1268,47 @@
         <v>2137168.514642729</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>0.84</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>37120</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>37120</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <f>C6*(1+(B6)/100)</f>
         <v>37431.807999999997</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <f t="shared" ref="F6:F8" si="0">E6</f>
         <v>37431.807999999997</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <f t="shared" ref="G6:G8" si="1">E6-D6</f>
         <v>311.80799999999726</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <f t="shared" ref="H6:H8" si="2">G6</f>
         <v>311.80799999999726</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="8">
         <v>0</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <f t="shared" ref="J6:J8" si="3">G6/((1.03)^2)</f>
         <v>293.90894523517511</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <f t="shared" ref="K6:K8" si="4">H6/((1.03)^3)</f>
         <v>285.34849051958747</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="8">
         <f t="shared" ref="L6:L9" si="5">K6+J6</f>
         <v>579.25743575476258</v>
       </c>
@@ -1326,47 +1324,47 @@
         <v>12529338.335375516</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>0.94</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>46810</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>46810</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f>C7*(1+(B7)/100)</f>
         <v>47250.014000000003</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>47250.014000000003</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <f t="shared" si="1"/>
         <v>440.01400000000285</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <f t="shared" si="2"/>
         <v>440.01400000000285</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <v>0</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <f t="shared" si="3"/>
         <v>414.75539636158248</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <f t="shared" si="4"/>
         <v>402.67514209862378</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="8">
         <f t="shared" si="5"/>
         <v>817.43053846020621</v>
       </c>
@@ -1382,47 +1380,47 @@
         <v>14305034.423053611</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>55640</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>55640</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <f>C8*(1+(B8)/100)</f>
         <v>55946.020000000004</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>55946.020000000004</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <f t="shared" si="1"/>
         <v>306.02000000000407</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <f t="shared" si="2"/>
         <v>306.02000000000407</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="8">
         <v>0</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <f t="shared" si="3"/>
         <v>288.45320011311537</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <f t="shared" si="4"/>
         <v>280.05165059525763</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="8">
         <f t="shared" si="5"/>
         <v>568.50485070837294</v>
       </c>
@@ -1438,7 +1436,7 @@
         <v>11580443.808929557</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1448,23 +1446,23 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <f>SUM(J5:J8)</f>
         <v>1188.3655386935666</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="9">
         <f>SUM(K5:K8)</f>
         <v>1153.7529501879285</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="8">
         <f t="shared" si="5"/>
         <v>2342.1184888814951</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <f>SUM(M5:M8)</f>
         <v>931</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="4">
         <f>SUM(N5:N8)</f>
         <v>579314072.60002017</v>
       </c>
@@ -1473,15 +1471,15 @@
         <v>40551985.082001418</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1503,38 +1501,35 @@
       <c r="H11" s="2">
         <v>55640</v>
       </c>
-      <c r="I11" s="5">
-        <f>F11/((1.03))</f>
-        <v>54019.417475728151</v>
-      </c>
-      <c r="J11" s="5">
+      <c r="I11" s="4"/>
+      <c r="J11" s="4">
         <f>G11/((1.03)^2)</f>
         <v>52446.036384202096</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <f>H11/((1.03)^2)</f>
         <v>52446.036384202096</v>
       </c>
       <c r="L11" s="3">
         <f>K11+J11+I11</f>
-        <v>158911.49024413235</v>
-      </c>
-      <c r="M11" s="6">
-        <v>9.3000000000000007</v>
+        <v>104892.07276840419</v>
+      </c>
+      <c r="M11" s="5">
+        <v>7</v>
       </c>
       <c r="N11" s="3">
         <f>M11*L11*1000</f>
-        <v>1477876859.2704308</v>
+        <v>734244509.37882936</v>
       </c>
       <c r="O11" s="3">
         <f t="shared" si="7"/>
-        <v>103451380.14893016</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>51397115.656518057</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I12" s="2">
         <f>SUM(I9:I11)</f>
-        <v>54019.417475728151</v>
+        <v>0</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" ref="J12:L12" si="8">SUM(J9:J11)</f>
@@ -1546,18 +1541,19 @@
       </c>
       <c r="L12" s="2">
         <f t="shared" si="8"/>
-        <v>161253.60873301385</v>
+        <v>107234.19125728568</v>
       </c>
       <c r="M12" s="2"/>
-      <c r="N12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O12" s="5">
+      <c r="N12" s="4">
+        <f>N11+N9</f>
+        <v>1313558581.9788494</v>
+      </c>
+      <c r="O12" s="4">
         <f>O11+O9</f>
-        <v>144003365.23093158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+        <v>91949100.738519475</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
@@ -1574,138 +1570,138 @@
       <c r="F16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>26350</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>26350</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <v>26552.895</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>26552.895</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>376.92566395815322</v>
       </c>
       <c r="G17" s="1">
         <v>81</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <v>30530978.780610409</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="8">
         <v>2137168.514642729</v>
       </c>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>37120</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>37120</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="7">
         <v>37431.807999999997</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="7">
         <v>37431.807999999997</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>579.25743575476258</v>
       </c>
       <c r="G18" s="1">
         <v>309</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>178990547.64822164</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="8">
         <v>12529338.335375516</v>
       </c>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>46810</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>46810</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <v>47250.014000000003</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="7">
         <v>47250.014000000003</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>817.43053846020621</v>
       </c>
       <c r="G19" s="1">
         <v>250</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>204357634.61505157</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="8">
         <v>14305034.423053611</v>
       </c>
-      <c r="J19" s="10"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>55640</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>55640</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>55946.020000000004</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>55946.020000000004</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>568.50485070837294</v>
       </c>
       <c r="G20" s="1">
         <v>291</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>165434911.55613652</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>11580443.808929557</v>
       </c>
-      <c r="J20" s="10"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1713,58 +1709,58 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <v>2342.1184888814951</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="12">
         <v>931</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="15">
         <v>579314072.60002017</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="8">
         <v>40551985.082001418</v>
       </c>
-      <c r="J21" s="10"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F22" s="3"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="7">
         <v>55640</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>55640</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="7">
         <v>55640</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>55640</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="8">
         <v>158911.49024413235</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <v>1477876859.2704308</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="8">
         <v>103451380.14893016</v>
       </c>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1772,17 +1768,17 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="8">
+      <c r="F24" s="7">
         <v>161253.60873301385</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="14">
         <v>940</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="9">
         <f>H23+H21</f>
         <v>2057190931.870451</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="15">
         <f>I23+I21</f>
         <v>144003365.23093158</v>
       </c>
@@ -1795,133 +1791,133 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDEF18D8-9DD6-1643-B576-A264E6854BC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>81</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <f>B5/B$9</f>
         <v>8.7003222341568209E-2</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="17">
         <v>81</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="16">
         <f>D5/D$9</f>
         <v>8.6353944562899784E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>309</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <f t="shared" ref="C6:E8" si="0">B6/B$9</f>
         <v>0.33190118152524167</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="17">
         <v>309</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <f t="shared" si="0"/>
         <v>0.32942430703624731</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>250</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <f t="shared" si="0"/>
         <v>0.26852846401718583</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="17">
         <v>250</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <f t="shared" si="0"/>
         <v>0.26652452025586354</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>291</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <f t="shared" si="0"/>
         <v>0.31256713211600429</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="17">
         <v>298</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <f t="shared" si="0"/>
         <v>0.31769722814498935</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <f>SUM(B5:B8)</f>
         <v>931</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="14">
+      <c r="C9" s="6"/>
+      <c r="D9" s="13">
         <f>SUM(D5:D8)</f>
         <v>938</v>
       </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>